<commit_message>
Atualizando descrição do Notebook
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23229"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E9802D4-A156-4C73-8830-B5AC4F7C6096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B894D89C-F9D3-4187-A476-6DC326D54C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,22 +48,22 @@
     <t>Na Embraer</t>
   </si>
   <si>
+    <t xml:space="preserve">Qual faculdade vocês faz? </t>
+  </si>
+  <si>
+    <t>Engenharia de Sistemas</t>
+  </si>
+  <si>
+    <t>Onde você mora?</t>
+  </si>
+  <si>
+    <t>Montes Claros - MG</t>
+  </si>
+  <si>
     <t>Onde você nasceu?</t>
   </si>
   <si>
     <t>Porteirinha - MG</t>
-  </si>
-  <si>
-    <t>Onde você mora?</t>
-  </si>
-  <si>
-    <t>Montes Claros - MG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qual faculdade vocês faz? </t>
-  </si>
-  <si>
-    <t>Engenharia de Sistemas</t>
   </si>
   <si>
     <t>Qual sua área de interesse?</t>
@@ -424,7 +424,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>